<commit_message>
Include Eingliederungszuschuss in KG
</commit_message>
<xml_diff>
--- a/knowledge_graph/ontology/vocabulary_list.xlsx
+++ b/knowledge_graph/ontology/vocabulary_list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Data graph" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="87">
   <si>
     <t xml:space="preserve">IRI</t>
   </si>
@@ -63,19 +63,37 @@
     <t xml:space="preserve">ff:MaritalStatus</t>
   </si>
   <si>
-    <t xml:space="preserve">ff:single</t>
-  </si>
-  <si>
-    <t xml:space="preserve">disjoint of married, disjoint of registeredPartnership</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ff:married</t>
-  </si>
-  <si>
-    <t xml:space="preserve">disjoint of registeredPartnership</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ff:reigsteredPartnership</t>
+    <t xml:space="preserve">ff:Single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disjoint of Married, disjoint of RegisteredPartnershi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff:Married</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disjoint of RegisteredPartnership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff:RegisteredPartnership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff:Performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff:AveragePerformance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disjoint of BeloAveragePerformance, AboveAveragePerformance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff:BelowAveragePerformance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disjoint of AboveAveragePreformance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff:AboveAveragePerformance</t>
   </si>
   <si>
     <t xml:space="preserve">OBJECT PROPERTIES</t>
@@ -102,6 +120,12 @@
     <t xml:space="preserve">symmetric</t>
   </si>
   <si>
+    <t xml:space="preserve">ff:expectedPerformance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff:Person → ff:Performance</t>
+  </si>
+  <si>
     <t xml:space="preserve">DATA PROPERTIES</t>
   </si>
   <si>
@@ -126,6 +150,9 @@
     <t xml:space="preserve">ff:checkedPriorityClaims</t>
   </si>
   <si>
+    <t xml:space="preserve">ff:integrationRequiresSubsidy</t>
+  </si>
+  <si>
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
@@ -177,19 +204,82 @@
     <t xml:space="preserve">ff:PriorityClaimsProperty</t>
   </si>
   <si>
+    <t xml:space="preserve">Person → Literal (int)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Person → MaritalStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff:Single </t>
+  </si>
+  <si>
+    <t xml:space="preserve">subclass of ff:MaritalStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Implied, subclass of ff:MaritalStatus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implied</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Person → Person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amount of child benefit a child receives in euros</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Person → Literal (bool)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ff:bruttoIncome</t>
   </si>
   <si>
+    <t xml:space="preserve">Person → Literal (float)</t>
+  </si>
+  <si>
     <t xml:space="preserve">ff:NonExistentPath</t>
   </si>
   <si>
-    <t xml:space="preserve">ff:EmployeeProperty</t>
+    <t xml:space="preserve">always invalid, always triggers warning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subclass of ff:Person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff:ProspectiveEmployeeProperty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">checks if prospective employee has below average expected performance and requires subsidy to be integrated long term</t>
   </si>
   <si>
     <t xml:space="preserve">ff:Eingliederungszuschuss</t>
   </si>
   <si>
-    <t xml:space="preserve">B</t>
+    <t xml:space="preserve">subclass of ff:FundingProgram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff:EingliederungszuschussShape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff:wantsToEmploy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff:Employer → ff:Person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff:expectedPeformance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subclass of ff:Performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">implied, subclass of ff:Performance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff:AboveAveragePerformace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ff:Employee → Literal (boolean)</t>
   </si>
   <si>
     <t xml:space="preserve">The ontology is intended to conceptualize social service descriptions from the perspective of user profiles. It is not intended to capture the logic of the SHACL shapes graphs derived from the social service descriptions. Thus, when passing the ontology as context to an LLM, it can reuse the datafields that serve as building blocks for user profiles (otherwise we could not control the modelling depth and no meaningful comparison or validation would be possible) but it cannot simply copy the constraint logic used in the groundtruth.</t>
@@ -202,7 +292,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -259,6 +349,18 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF666666"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -276,7 +378,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF2A6099"/>
-        <bgColor rgb="FF666699"/>
+        <bgColor rgb="FF158466"/>
       </patternFill>
     </fill>
     <fill>
@@ -332,7 +434,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -373,6 +475,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -398,6 +504,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -462,7 +576,7 @@
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF666666"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -588,10 +702,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G1023"/>
+  <dimension ref="A1:G1027"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B24" activeCellId="0" sqref="B24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.94921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -729,83 +843,102 @@
       </c>
     </row>
     <row r="11" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="C11" s="9"/>
+      <c r="F11" s="0" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="12" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="8" t="s">
+        <v>18</v>
+      </c>
       <c r="C12" s="9"/>
-    </row>
-    <row r="13" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="10" t="s">
+      <c r="F12" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" s="1" customFormat="true" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-    </row>
-    <row r="14" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C13" s="9"/>
+      <c r="D13" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" s="1" customFormat="true" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="9"/>
+      <c r="D14" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F14" s="0" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="15" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="F15" s="0" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="16" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="12"/>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="9"/>
+    </row>
+    <row r="17" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C17" s="9"/>
+    </row>
+    <row r="18" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E16" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="12"/>
-    </row>
-    <row r="18" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="12"/>
-    </row>
-    <row r="19" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="13" t="s">
+      <c r="B19" s="13"/>
+      <c r="C19" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14"/>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
+      <c r="E19" s="8" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="12"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="8" t="s">
         <v>28</v>
       </c>
@@ -813,49 +946,119 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="B21" s="12"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="8" t="s">
         <v>30</v>
       </c>
+      <c r="D21" s="8" t="s">
+        <v>31</v>
+      </c>
       <c r="E21" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="22" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="12"/>
+        <v>32</v>
+      </c>
+      <c r="B22" s="13"/>
       <c r="C22" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B23" s="12"/>
-      <c r="C23" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="24" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="25" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="26" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="27" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="28" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="29" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="30" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="31" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="32" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="33" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="F22" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="13"/>
+    </row>
+    <row r="24" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="13"/>
+    </row>
+    <row r="25" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="13"/>
+    </row>
+    <row r="26" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+    </row>
+    <row r="27" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27" s="13"/>
+      <c r="C27" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" s="13"/>
+      <c r="C29" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="13"/>
+      <c r="C30" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F30" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" s="1" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B31" s="13"/>
+      <c r="C31" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="F31" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="13"/>
+    </row>
+    <row r="33" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="13"/>
+    </row>
     <row r="34" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="35" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="36" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1846,6 +2049,10 @@
     <row r="1021" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1022" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1023" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1024" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1025" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1026" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1027" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -1862,10 +2069,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E1048576"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="32.43359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1874,23 +2081,23 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="C1" s="15" t="s">
+      <c r="B1" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="16"/>
+      <c r="E1" s="17"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>8</v>
@@ -1901,7 +2108,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>8</v>
@@ -1912,7 +2119,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="C4" s="8" t="s">
         <v>8</v>
@@ -1923,7 +2130,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>8</v>
@@ -1934,7 +2141,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>8</v>
@@ -1956,7 +2163,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>8</v>
@@ -1964,7 +2171,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>8</v>
@@ -1972,10 +2179,10 @@
     </row>
     <row r="10" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>43</v>
+        <v>52</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>8</v>
@@ -1983,7 +2190,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>8</v>
@@ -1991,7 +2198,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="8" t="s">
-        <v>44</v>
+        <v>53</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>8</v>
@@ -1999,10 +2206,10 @@
     </row>
     <row r="13" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>8</v>
@@ -2010,10 +2217,10 @@
     </row>
     <row r="14" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="8" t="s">
-        <v>47</v>
+        <v>56</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>8</v>
@@ -2021,36 +2228,37 @@
     </row>
     <row r="15" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="8" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="B16" s="8"/>
+        <v>59</v>
+      </c>
       <c r="C16" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="8"/>
+        <v>41</v>
+      </c>
       <c r="C17" s="8" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="8" t="s">
-        <v>27</v>
+        <v>35</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>60</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>8</v>
@@ -2058,7 +2266,10 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="8" t="s">
-        <v>21</v>
+        <v>27</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>61</v>
       </c>
       <c r="C19" s="8" t="s">
         <v>8</v>
@@ -2066,31 +2277,43 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="8" t="s">
-        <v>23</v>
+        <v>62</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>63</v>
       </c>
       <c r="C20" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="8" t="s">
-        <v>29</v>
+    <row r="21" s="19" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>64</v>
       </c>
       <c r="C21" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="8" t="s">
-        <v>31</v>
+    <row r="22" s="19" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>64</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="8" t="s">
-        <v>51</v>
+    <row r="23" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>65</v>
       </c>
       <c r="C23" s="8" t="s">
         <v>8</v>
@@ -2098,46 +2321,177 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="8" t="s">
-        <v>52</v>
+        <v>29</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="C24" s="8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1" t="s">
+    <row r="25" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B29" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="64.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" s="19" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B36" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" s="19" customFormat="true" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -2166,8 +2520,8 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="77.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="17" t="s">
-        <v>56</v>
+      <c r="A1" s="20" t="s">
+        <v>86</v>
       </c>
     </row>
   </sheetData>

</xml_diff>